<commit_message>
[modify] upgrade Evaluate-Condition for inc, dec
</commit_message>
<xml_diff>
--- a/powershell/smart.xlsx
+++ b/powershell/smart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testcode\powershell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDCE048-EA8E-433C-8BF2-BE90852C66E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5B701D-5B97-47A4-BDFA-18C967B84F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28260" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
   <si>
     <t>customer</t>
   </si>
@@ -216,13 +216,34 @@
   </si>
   <si>
     <t>199:60</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>NVME_GEN</t>
+  </si>
+  <si>
+    <t>NVME_DELL</t>
+  </si>
+  <si>
+    <t>NVME_HP</t>
+  </si>
+  <si>
+    <t>inc;gt:4;lt:10</t>
+  </si>
+  <si>
+    <t>dec;inc;gt:4;lt:10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,10 +278,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,24 +617,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -638,15 +659,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1">
-        <v>0</v>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -661,15 +682,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -684,334 +705,388 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1">
-        <v>3</v>
-      </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8">
+        <v>23</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8">
+        <v>32</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8">
+        <v>34</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>36</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H24" s="1"/>
+      <c r="H26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refactor Evaluate-Condition to use integer parameters and improve condition handling
</commit_message>
<xml_diff>
--- a/powershell/smart.xlsx
+++ b/powershell/smart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testcode\powershell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5B701D-5B97-47A4-BDFA-18C967B84F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7B01FB-24ED-4FFF-B2E6-468F18629958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28260" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -236,7 +236,7 @@
     <t>inc;gt:4;lt:10</t>
   </si>
   <si>
-    <t>dec;inc;gt:4;lt:10</t>
+    <t>dec;inc;gt:150;lt:10;ne;ne:2</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,7 @@
     <col min="3" max="3" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
refactor Compare-SmartData to use consistent variable naming and improve output clarity
</commit_message>
<xml_diff>
--- a/powershell/smart.xlsx
+++ b/powershell/smart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testcode\powershell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7B01FB-24ED-4FFF-B2E6-468F18629958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1133AB4-339D-4D47-B461-63A17909F464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28260" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="68">
   <si>
     <t>customer</t>
   </si>
@@ -47,9 +47,6 @@
     <t>byte_offset</t>
   </si>
   <si>
-    <t>criterai</t>
-  </si>
-  <si>
     <t>remark</t>
   </si>
   <si>
@@ -237,6 +234,12 @@
   </si>
   <si>
     <t>dec;inc;gt:150;lt:10;ne;ne:2</t>
+  </si>
+  <si>
+    <t>WARNING</t>
+  </si>
+  <si>
+    <t>criteria</t>
   </si>
 </sst>
 </file>
@@ -620,15 +623,16 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -644,447 +648,489 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
+      <c r="D8" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
+      <c r="D9" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>19</v>
+      <c r="D10" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>21</v>
+      <c r="D11" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>28</v>
+      <c r="D14" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="H26" s="1"/>
     </row>

</xml_diff>

<commit_message>
Add ImportExcel module and refactor Read-ExcelData function to support dynamic starting row
</commit_message>
<xml_diff>
--- a/powershell/smart.xlsx
+++ b/powershell/smart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testcode\powershell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1133AB4-339D-4D47-B461-63A17909F464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EE5F7F-789F-4232-9291-02DC4146621E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28260" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -620,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A3:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,104 +637,58 @@
     <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>44</v>
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -757,66 +711,82 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>66</v>
@@ -825,13 +795,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>66</v>
@@ -840,71 +810,55 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -912,40 +866,56 @@
         <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H15" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>66</v>
@@ -954,112 +924,104 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>32</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>51</v>
+        <v>14</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>52</v>
+        <v>30</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H19" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>53</v>
+        <v>33</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H20" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>35</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>66</v>
@@ -1068,54 +1030,54 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H23" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="H25" s="1"/>
     </row>
@@ -1124,15 +1086,53 @@
         <v>39</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H26" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Load PowerShell scripts from the Public directory in ImportExcel module
</commit_message>
<xml_diff>
--- a/powershell/smart.xlsx
+++ b/powershell/smart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testcode\powershell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EE5F7F-789F-4232-9291-02DC4146621E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5AC09E-933D-4422-AF66-EE079F4C91BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28260" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,51 +77,30 @@
     <t>criteria warining 5</t>
   </si>
   <si>
-    <t>5:4</t>
-  </si>
-  <si>
     <t>reserved</t>
   </si>
   <si>
-    <t>511:6</t>
-  </si>
-  <si>
     <t>DELL</t>
   </si>
   <si>
     <t>criteria warining 7</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>criteria warining 8</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>criteria warining 9</t>
   </si>
   <si>
-    <t>5:2</t>
-  </si>
-  <si>
     <t>criteria warining 10</t>
   </si>
   <si>
-    <t>10:6</t>
-  </si>
-  <si>
     <t>eq:100</t>
   </si>
   <si>
     <t>criteria warining 11</t>
   </si>
   <si>
-    <t>99:11</t>
-  </si>
-  <si>
     <t>criteria warining 12</t>
   </si>
   <si>
@@ -131,9 +110,6 @@
     <t>criteria warining 14</t>
   </si>
   <si>
-    <t>3:0</t>
-  </si>
-  <si>
     <t>inc</t>
   </si>
   <si>
@@ -191,36 +167,6 @@
     <t>511:200</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>9:6</t>
-  </si>
-  <si>
-    <t>19:10</t>
-  </si>
-  <si>
-    <t>29:20</t>
-  </si>
-  <si>
-    <t>39:30</t>
-  </si>
-  <si>
-    <t>59:40</t>
-  </si>
-  <si>
-    <t>199:60</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>NVME_GEN</t>
   </si>
   <si>
@@ -240,6 +186,60 @@
   </si>
   <si>
     <t>criteria</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>005:004</t>
+  </si>
+  <si>
+    <t>511:006</t>
+  </si>
+  <si>
+    <t>005:002</t>
+  </si>
+  <si>
+    <t>010:006</t>
+  </si>
+  <si>
+    <t>099:011</t>
+  </si>
+  <si>
+    <t>003:000</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>009:006</t>
+  </si>
+  <si>
+    <t>019:010</t>
+  </si>
+  <si>
+    <t>029:020</t>
+  </si>
+  <si>
+    <t>039:030</t>
+  </si>
+  <si>
+    <t>059:040</t>
+  </si>
+  <si>
+    <t>199:060</t>
   </si>
 </sst>
 </file>
@@ -623,7 +623,7 @@
   <dimension ref="A3:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,19 +648,19 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -671,7 +671,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -688,71 +688,71 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -763,10 +763,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>10</v>
@@ -786,10 +786,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -801,10 +801,10 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="H10" s="1"/>
     </row>
@@ -813,324 +813,324 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C13" s="3" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="H28" s="1"/>
     </row>

</xml_diff>